<commit_message>
Fix search for sales person and account manager.
1. Replacing 'concat' function with concatenation operator (||). qa/stage/prod postgres db version is 8.4 which does not support 'concat' function to concatenate string. 
2. Updated io fixture file with correct email of Eric Burns
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO.xlsx
+++ b/spec/fixtures/io_files/Collective_IO.xlsx
@@ -20,15 +20,18 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" name="Network" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="174">
   <si>
     <t>Date:</t>
   </si>
@@ -71,19 +74,16 @@
     <t>919-604-4451</t>
   </si>
   <si>
-    <t>Phone: </t>
-  </si>
-  <si>
     <t>646-786-6701</t>
   </si>
   <si>
     <t>646-442-8220</t>
   </si>
   <si>
-    <t>Email: </t>
-  </si>
-  <si>
-    <t>eric@collective.com</t>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>eburns@collective.com</t>
   </si>
   <si>
     <t>ampnetwork@collective.com</t>
@@ -98,7 +98,7 @@
     <t>AMP Network CORE</t>
   </si>
   <si>
-    <t>Media Contact: </t>
+    <t>Media Contact:</t>
   </si>
   <si>
     <t>Mary Ball</t>
@@ -116,15 +116,12 @@
     <t>Otterbein University</t>
   </si>
   <si>
-    <t>Company: </t>
+    <t>Company:</t>
   </si>
   <si>
     <t>Time Warner Cable</t>
   </si>
   <si>
-    <t>Company:</t>
-  </si>
-  <si>
     <t>Order Name:</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>digital.services@twcable.com</t>
   </si>
   <si>
-    <t>Email:</t>
-  </si>
-  <si>
     <t>Campaign Start:</t>
   </si>
   <si>
@@ -188,13 +182,13 @@
     <t>RON; Columbus Zips</t>
   </si>
   <si>
-    <t>Totals: </t>
-  </si>
-  <si>
-    <t>NOTES:  </t>
-  </si>
-  <si>
-    <t>Deliver Evenly.  </t>
+    <t>Totals:</t>
+  </si>
+  <si>
+    <t>NOTES:</t>
+  </si>
+  <si>
+    <t>Deliver Evenly.</t>
   </si>
   <si>
     <t>Delivery:</t>
@@ -209,7 +203,7 @@
     <t>Payment terms:</t>
   </si>
   <si>
-    <t>Net 30 Days.   </t>
+    <t>Net 30 Days.</t>
   </si>
   <si>
     <t>Terms &amp; Conditions:</t>
@@ -242,15 +236,12 @@
     <t>Authorized Signature Advertiser</t>
   </si>
   <si>
-    <t>                Date</t>
+    <t>Date</t>
   </si>
   <si>
     <t>Collective Media</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>Internal Redirects</t>
   </si>
   <si>
@@ -357,9 +348,6 @@
   </si>
   <si>
     <t>Additional Info.</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t>Collective Ad Network</t>
@@ -538,8 +526,7 @@
   </si>
   <si>
     <t>FLV (at least Flash 7), MOV and WMV
-(if possible -- but FLV and MOV are necessary) 
-</t>
+(if possible -- but FLV and MOV are necessary)</t>
   </si>
   <si>
     <t>480x360</t>
@@ -576,8 +563,7 @@
   </si>
   <si>
     <t>FLV (at least Flash 7), MOV and WMV 
-(if possible -- but FLV and MOV are necessary) 
-</t>
+(if possible -- but FLV and MOV are necessary)</t>
   </si>
   <si>
     <t>480x270</t>
@@ -597,7 +583,7 @@
     <numFmt formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)" numFmtId="170"/>
     <numFmt formatCode="@" numFmtId="171"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="26">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -669,11 +655,6 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <charset val="1"/>
       <family val="2"/>
@@ -682,18 +663,21 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="8"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="FF0000FF"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="FF0000D4"/>
       <sz val="8"/>
@@ -713,12 +697,6 @@
       <b val="true"/>
       <sz val="10"/>
       <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="8"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -919,7 +897,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="22">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -954,32 +932,8 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="126">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1076,15 +1030,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="11" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1112,7 +1062,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1120,15 +1070,15 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1136,39 +1086,27 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="12" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="14" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="9" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="11" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="14" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="3" fontId="15" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="16" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1176,7 +1114,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="17" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1188,11 +1126,11 @@
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="11" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="17" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1216,23 +1154,19 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="11" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="11" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="0" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1244,30 +1178,14 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="2" fontId="11" numFmtId="165" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="11" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="5" fillId="2" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="4" fillId="2" fontId="0" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="false"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
@@ -1280,7 +1198,7 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="18" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="12" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1288,23 +1206,23 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="19" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="17" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="2" fontId="19" numFmtId="165" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="2" fillId="2" fontId="17" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="19" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="19" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="17" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="20" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
@@ -1368,7 +1286,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="21" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="19" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1376,7 +1294,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="22" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="0" fontId="20" numFmtId="164" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1400,7 +1318,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1424,7 +1342,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="21">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1436,35 +1354,35 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="26" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="27" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="24" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="24" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1480,27 +1398,27 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="25" numFmtId="171" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="171" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="26" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="24" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1508,34 +1426,28 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="20">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="25" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="8">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2" xfId="21"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 2" xfId="22"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 2 2" xfId="23"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 3" xfId="24"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 3 2" xfId="25"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 4" xfId="26"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Normal 2 4 2" xfId="27"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1605,15 +1517,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>131760</xdr:colOff>
+      <xdr:colOff>158760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76680</xdr:rowOff>
+      <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>365040</xdr:colOff>
+      <xdr:colOff>391680</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1628,8 +1540,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="131760" y="219240"/>
-          <a:ext cx="1231200" cy="599760"/>
+          <a:off x="158760" y="210240"/>
+          <a:ext cx="1230840" cy="599400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,15 +1553,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1255320</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:colOff>1281960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1658,8 +1570,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="57600"/>
-          <a:ext cx="12355200" cy="47160"/>
+          <a:off x="54000" y="48600"/>
+          <a:ext cx="12354840" cy="46800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1680,15 +1592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1255320</xdr:colOff>
+      <xdr:colOff>1281960</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1697,8 +1609,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="886320"/>
-          <a:ext cx="12355200" cy="47160"/>
+          <a:off x="54000" y="877320"/>
+          <a:ext cx="12354840" cy="46800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1719,15 +1631,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>7560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1293480</xdr:colOff>
+      <xdr:colOff>1320120</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>149760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1736,8 +1648,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="6218280"/>
-          <a:ext cx="12393360" cy="142560"/>
+          <a:off x="54000" y="6209280"/>
+          <a:ext cx="12393000" cy="142200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1758,15 +1670,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1284120</xdr:colOff>
+      <xdr:colOff>1310760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>42840</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1775,8 +1687,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="2972160"/>
-          <a:ext cx="12384000" cy="45360"/>
+          <a:off x="54000" y="2963160"/>
+          <a:ext cx="12383640" cy="45000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1802,15 +1714,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>84240</xdr:colOff>
+      <xdr:colOff>111240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>150480</xdr:colOff>
+      <xdr:colOff>177120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>248040</xdr:rowOff>
+      <xdr:rowOff>238680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1825,8 +1737,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="84240" y="48240"/>
-          <a:ext cx="1597680" cy="723600"/>
+          <a:off x="111240" y="39240"/>
+          <a:ext cx="1597320" cy="723240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1843,15 +1755,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>131760</xdr:colOff>
+      <xdr:colOff>158760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>198000</xdr:colOff>
+      <xdr:colOff>224640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>305280</xdr:rowOff>
+      <xdr:rowOff>295920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1866,8 +1778,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="131760" y="105480"/>
-          <a:ext cx="1597680" cy="723600"/>
+          <a:off x="158760" y="96480"/>
+          <a:ext cx="1597320" cy="723240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1884,15 +1796,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>131760</xdr:colOff>
+      <xdr:colOff>158760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>198000</xdr:colOff>
+      <xdr:colOff>224640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:rowOff>248040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1907,8 +1819,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="131760" y="57600"/>
-          <a:ext cx="1597680" cy="723600"/>
+          <a:off x="158760" y="48600"/>
+          <a:ext cx="1597320" cy="723240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1928,7 +1840,7 @@
   <dimension ref="A1:AI181"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E22" activeCellId="0" pane="topLeft" sqref="E22"/>
+      <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2345,63 +2257,63 @@
       <c r="D12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="27"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13" s="5">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29" t="s">
+      <c r="B13" s="27"/>
+      <c r="C13" s="28" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>11</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14" s="5">
+      <c r="A14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="27"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14" s="5">
-      <c r="A14" s="28" t="s">
+      <c r="B14" s="27"/>
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="27"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="26"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15" s="5">
       <c r="A15" s="7"/>
@@ -2413,127 +2325,127 @@
       <c r="G15" s="2"/>
       <c r="H15" s="6"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="27"/>
+      <c r="J15" s="26"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="16" s="5">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="31"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="7"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="2"/>
       <c r="H16" s="6"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="27"/>
+      <c r="J16" s="26"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="17" s="5">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33" t="s">
+      <c r="D17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="E17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="F17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="G17" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="H17" s="35"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="18" s="5">
+      <c r="A18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="36"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="18" s="5">
-      <c r="A18" s="32" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="35"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="26.25" outlineLevel="0" r="19" s="5">
+      <c r="A19" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="B19" s="38"/>
+      <c r="C19" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="39"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="26.25" outlineLevel="0" r="19" s="5">
-      <c r="A19" s="40" t="s">
+      <c r="D19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20" s="5">
+      <c r="A20" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="40" t="n">
+        <v>7762936</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="37" t="s">
         <v>30</v>
-      </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.5" outlineLevel="0" r="20" s="5">
-      <c r="A20" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="43" t="n">
-        <v>7762936</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>32</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="36"/>
+      <c r="G20" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="21" s="5">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="45" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>32</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="46"/>
+        <v>12</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="42"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="22" s="6">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="38"/>
       <c r="C22" s="3"/>
-      <c r="H22" s="47"/>
+      <c r="H22" s="43"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -2582,43 +2494,43 @@
       <c r="E24" s="2"/>
       <c r="F24" s="3"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="48"/>
+      <c r="H24" s="44"/>
       <c r="I24" s="1"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="25" s="5">
-      <c r="A25" s="49"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="50"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="52" t="n">
+      <c r="G25" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="48" t="n">
         <v>41503</v>
       </c>
-      <c r="I25" s="29"/>
+      <c r="I25" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="26" s="5">
-      <c r="A26" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54" t="n">
+      <c r="A26" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50" t="n">
         <f aca="false">H40</f>
         <v>0</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="52" t="n">
+      <c r="G26" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="48" t="n">
         <v>41515</v>
       </c>
-      <c r="I26" s="29"/>
+      <c r="I26" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="8.1" outlineLevel="0" r="27" s="6">
       <c r="A27" s="2"/>
@@ -2628,8 +2540,8 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="29"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="28"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2658,29 +2570,29 @@
       <c r="AI27" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="28" s="6">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="57" t="s">
+      <c r="E28" s="52"/>
+      <c r="F28" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="58" t="s">
+      <c r="G28" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="56" t="s">
+      <c r="H28" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" s="56" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="I28" s="29"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -2709,166 +2621,166 @@
       <c r="AI28" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="29" s="5">
-      <c r="A29" s="59" t="n">
+      <c r="A29" s="55" t="n">
         <v>41503</v>
       </c>
-      <c r="B29" s="60" t="n">
+      <c r="B29" s="55" t="n">
         <v>41515</v>
       </c>
-      <c r="C29" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63" t="n">
+      <c r="C29" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58" t="n">
         <v>300000</v>
       </c>
-      <c r="G29" s="64"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="29"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="30" s="5">
-      <c r="A30" s="66" t="n">
+      <c r="A30" s="61" t="n">
         <v>41503</v>
       </c>
-      <c r="B30" s="66" t="n">
+      <c r="B30" s="61" t="n">
         <v>41515</v>
       </c>
-      <c r="C30" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="67" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="67"/>
-      <c r="F30" s="63" t="n">
+      <c r="C30" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="62"/>
+      <c r="F30" s="58" t="n">
         <v>210000</v>
       </c>
-      <c r="G30" s="64"/>
-      <c r="H30" s="65"/>
-      <c r="I30" s="29"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="31" s="5">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="29"/>
+      <c r="A31" s="61"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="32" s="5">
-      <c r="A32" s="68"/>
-      <c r="B32" s="68"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="29"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="33" s="5">
-      <c r="A33" s="68"/>
-      <c r="B33" s="68"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="29"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="34" s="5">
-      <c r="A34" s="68"/>
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="29"/>
+      <c r="A34" s="61"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="35" s="5">
-      <c r="A35" s="68"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="29"/>
+      <c r="A35" s="61"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="36" s="5">
-      <c r="A36" s="73"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="65"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="65"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="60"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37" s="5">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="65"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="60"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="38" s="5">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39" s="81">
-      <c r="A39" s="77"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="65"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="67"/>
+      <c r="H38" s="60"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="39" s="72">
+      <c r="A39" s="68"/>
+      <c r="B39" s="69"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="60"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="40" s="5">
-      <c r="A40" s="82" t="s">
-        <v>49</v>
-      </c>
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="84" t="n">
+      <c r="A40" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="75" t="n">
         <f aca="false">SUM(F29:F39)</f>
         <v>510000</v>
       </c>
-      <c r="G40" s="85" t="n">
+      <c r="G40" s="76" t="n">
         <f aca="false">H40/F40*1000</f>
         <v>0</v>
       </c>
-      <c r="H40" s="86" t="n">
+      <c r="H40" s="77" t="n">
         <f aca="false">SUM(H29:H39)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="41" s="6">
       <c r="A41" s="2"/>
@@ -2908,18 +2820,18 @@
       <c r="AI41" s="5"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="21.75" outlineLevel="0" r="42" s="5">
-      <c r="A42" s="87" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="88" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="88"/>
-      <c r="H42" s="88"/>
+      <c r="A42" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="79"/>
+      <c r="D42" s="79"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43" s="6">
       <c r="A43" s="2"/>
@@ -3001,9 +2913,9 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="29"/>
+      <c r="F45" s="28"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="48"/>
+      <c r="H45" s="44"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46" s="5">
       <c r="A46" s="1"/>
@@ -3016,242 +2928,242 @@
       <c r="H46" s="1"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="47" s="5">
-      <c r="A47" s="89" t="s">
+      <c r="A47" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="81"/>
+      <c r="C47" s="82" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="81"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="81"/>
+      <c r="G47" s="81"/>
+      <c r="H47" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="48" s="5">
+      <c r="A48" s="80"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="81"/>
+      <c r="E48" s="81"/>
+      <c r="F48" s="81"/>
+      <c r="G48" s="81"/>
+      <c r="H48" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="49" s="5">
+      <c r="A49" s="81"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="81"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="81"/>
+      <c r="G49" s="81"/>
+      <c r="H49" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50" s="5">
+      <c r="A50" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="91" t="s">
+      <c r="B50" s="81"/>
+      <c r="C50" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="90"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="90"/>
-      <c r="H47" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="48" s="5">
-      <c r="A48" s="89"/>
-      <c r="B48" s="90"/>
-      <c r="C48" s="91" t="s">
+      <c r="D50" s="81"/>
+      <c r="E50" s="81"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="81"/>
+      <c r="H50" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51" s="5">
+      <c r="A51" s="81"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="81"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
+      <c r="F51" s="81"/>
+      <c r="G51" s="81"/>
+      <c r="H51" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="52" s="5">
+      <c r="A52" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="90"/>
-      <c r="G48" s="90"/>
-      <c r="H48" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="49" s="5">
-      <c r="A49" s="90"/>
-      <c r="B49" s="90"/>
-      <c r="C49" s="90"/>
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="90"/>
-      <c r="G49" s="90"/>
-      <c r="H49" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50" s="5">
-      <c r="A50" s="91" t="s">
+      <c r="B52" s="81"/>
+      <c r="C52" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="90"/>
-      <c r="C50" s="91" t="s">
+      <c r="D52" s="83"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
+      <c r="H52" s="83"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="53" s="5">
+      <c r="A53" s="81"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="83"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="83"/>
+      <c r="G53" s="83"/>
+      <c r="H53" s="83"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="54" s="5">
+      <c r="A54" s="81"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="84"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="84"/>
+      <c r="F54" s="84"/>
+      <c r="G54" s="84"/>
+      <c r="H54" s="84"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="55" s="5">
+      <c r="A55" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51" s="5">
-      <c r="A51" s="90"/>
-      <c r="B51" s="90"/>
-      <c r="C51" s="90"/>
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="90"/>
-      <c r="G51" s="90"/>
-      <c r="H51" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="52" s="5">
-      <c r="A52" s="91" t="s">
+      <c r="B55" s="82"/>
+      <c r="C55" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="90"/>
-      <c r="C52" s="92" t="s">
+      <c r="D55" s="85"/>
+      <c r="E55" s="85"/>
+      <c r="F55" s="85"/>
+      <c r="G55" s="85"/>
+      <c r="H55" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="56" s="5">
+      <c r="A56" s="82"/>
+      <c r="B56" s="82"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+      <c r="F56" s="85"/>
+      <c r="G56" s="85"/>
+      <c r="H56" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="57" s="5">
+      <c r="A57" s="82"/>
+      <c r="B57" s="82"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="85"/>
+      <c r="F57" s="85"/>
+      <c r="G57" s="85"/>
+      <c r="H57" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="58" s="5">
+      <c r="A58" s="82"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="86"/>
+      <c r="H58" s="86"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="59" s="5">
+      <c r="A59" s="82" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="92"/>
-      <c r="E52" s="92"/>
-      <c r="F52" s="92"/>
-      <c r="G52" s="92"/>
-      <c r="H52" s="92"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="53" s="5">
-      <c r="A53" s="90"/>
-      <c r="B53" s="90"/>
-      <c r="C53" s="92"/>
-      <c r="D53" s="92"/>
-      <c r="E53" s="92"/>
-      <c r="F53" s="92"/>
-      <c r="G53" s="92"/>
-      <c r="H53" s="92"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="54" s="5">
-      <c r="A54" s="90"/>
-      <c r="B54" s="90"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="93"/>
-      <c r="E54" s="93"/>
-      <c r="F54" s="93"/>
-      <c r="G54" s="93"/>
-      <c r="H54" s="93"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="55" s="5">
-      <c r="A55" s="91" t="s">
+      <c r="B59" s="82"/>
+      <c r="C59" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="91"/>
-      <c r="C55" s="94" t="s">
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="60" s="5">
+      <c r="A60" s="82"/>
+      <c r="B60" s="82"/>
+      <c r="C60" s="85"/>
+      <c r="D60" s="85"/>
+      <c r="E60" s="85"/>
+      <c r="F60" s="85"/>
+      <c r="G60" s="85"/>
+      <c r="H60" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="61" s="5">
+      <c r="A61" s="82"/>
+      <c r="B61" s="82"/>
+      <c r="C61" s="85"/>
+      <c r="D61" s="85"/>
+      <c r="E61" s="85"/>
+      <c r="F61" s="85"/>
+      <c r="G61" s="85"/>
+      <c r="H61" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="62" s="5">
+      <c r="A62" s="82"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86"/>
+      <c r="G62" s="86"/>
+      <c r="H62" s="86"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="63" s="5">
+      <c r="A63" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="D55" s="94"/>
-      <c r="E55" s="94"/>
-      <c r="F55" s="94"/>
-      <c r="G55" s="94"/>
-      <c r="H55" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="56" s="5">
-      <c r="A56" s="91"/>
-      <c r="B56" s="91"/>
-      <c r="C56" s="94"/>
-      <c r="D56" s="94"/>
-      <c r="E56" s="94"/>
-      <c r="F56" s="94"/>
-      <c r="G56" s="94"/>
-      <c r="H56" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="57" s="5">
-      <c r="A57" s="91"/>
-      <c r="B57" s="91"/>
-      <c r="C57" s="94"/>
-      <c r="D57" s="94"/>
-      <c r="E57" s="94"/>
-      <c r="F57" s="94"/>
-      <c r="G57" s="94"/>
-      <c r="H57" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="58" s="5">
-      <c r="A58" s="91"/>
-      <c r="B58" s="91"/>
-      <c r="C58" s="95"/>
-      <c r="D58" s="95"/>
-      <c r="E58" s="95"/>
-      <c r="F58" s="95"/>
-      <c r="G58" s="95"/>
-      <c r="H58" s="95"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="59" s="5">
-      <c r="A59" s="91" t="s">
+      <c r="B63" s="82"/>
+      <c r="C63" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B59" s="91"/>
-      <c r="C59" s="94" t="s">
+      <c r="D63" s="85"/>
+      <c r="E63" s="85"/>
+      <c r="F63" s="85"/>
+      <c r="G63" s="85"/>
+      <c r="H63" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="64" s="5">
+      <c r="A64" s="82"/>
+      <c r="B64" s="82"/>
+      <c r="C64" s="85"/>
+      <c r="D64" s="85"/>
+      <c r="E64" s="85"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="65" s="5">
+      <c r="A65" s="82"/>
+      <c r="B65" s="82"/>
+      <c r="C65" s="85"/>
+      <c r="D65" s="85"/>
+      <c r="E65" s="85"/>
+      <c r="F65" s="85"/>
+      <c r="G65" s="85"/>
+      <c r="H65" s="85"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="66" s="5">
+      <c r="A66" s="81"/>
+      <c r="B66" s="81"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
+      <c r="F66" s="81"/>
+      <c r="G66" s="81"/>
+      <c r="H66" s="81"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="67" s="5">
+      <c r="A67" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="D59" s="94"/>
-      <c r="E59" s="94"/>
-      <c r="F59" s="94"/>
-      <c r="G59" s="94"/>
-      <c r="H59" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="60" s="5">
-      <c r="A60" s="91"/>
-      <c r="B60" s="91"/>
-      <c r="C60" s="94"/>
-      <c r="D60" s="94"/>
-      <c r="E60" s="94"/>
-      <c r="F60" s="94"/>
-      <c r="G60" s="94"/>
-      <c r="H60" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="61" s="5">
-      <c r="A61" s="91"/>
-      <c r="B61" s="91"/>
-      <c r="C61" s="94"/>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
-      <c r="F61" s="94"/>
-      <c r="G61" s="94"/>
-      <c r="H61" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="62" s="5">
-      <c r="A62" s="91"/>
-      <c r="B62" s="91"/>
-      <c r="C62" s="95"/>
-      <c r="D62" s="95"/>
-      <c r="E62" s="95"/>
-      <c r="F62" s="95"/>
-      <c r="G62" s="95"/>
-      <c r="H62" s="95"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="63" s="5">
-      <c r="A63" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63" s="91"/>
-      <c r="C63" s="94" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="94"/>
-      <c r="E63" s="94"/>
-      <c r="F63" s="94"/>
-      <c r="G63" s="94"/>
-      <c r="H63" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="64" s="5">
-      <c r="A64" s="91"/>
-      <c r="B64" s="91"/>
-      <c r="C64" s="94"/>
-      <c r="D64" s="94"/>
-      <c r="E64" s="94"/>
-      <c r="F64" s="94"/>
-      <c r="G64" s="94"/>
-      <c r="H64" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="65" s="5">
-      <c r="A65" s="91"/>
-      <c r="B65" s="91"/>
-      <c r="C65" s="94"/>
-      <c r="D65" s="94"/>
-      <c r="E65" s="94"/>
-      <c r="F65" s="94"/>
-      <c r="G65" s="94"/>
-      <c r="H65" s="94"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="66" s="5">
-      <c r="A66" s="90"/>
-      <c r="B66" s="90"/>
-      <c r="C66" s="90"/>
-      <c r="D66" s="90"/>
-      <c r="E66" s="90"/>
-      <c r="F66" s="90"/>
-      <c r="G66" s="90"/>
-      <c r="H66" s="90"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="67" s="5">
-      <c r="A67" s="91" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="91"/>
-      <c r="C67" s="91"/>
-      <c r="D67" s="91"/>
-      <c r="E67" s="91"/>
-      <c r="F67" s="91"/>
-      <c r="G67" s="90"/>
-      <c r="H67" s="90"/>
+      <c r="B67" s="82"/>
+      <c r="C67" s="82"/>
+      <c r="D67" s="82"/>
+      <c r="E67" s="82"/>
+      <c r="F67" s="82"/>
+      <c r="G67" s="81"/>
+      <c r="H67" s="81"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="68" s="5">
       <c r="A68" s="1"/>
@@ -3284,28 +3196,28 @@
       <c r="H70" s="1"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="71" s="5">
-      <c r="A71" s="96"/>
-      <c r="B71" s="96"/>
-      <c r="C71" s="96"/>
-      <c r="D71" s="96"/>
+      <c r="A71" s="87"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="87"/>
+      <c r="D71" s="87"/>
       <c r="E71" s="8"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="96"/>
-      <c r="H71" s="96"/>
+      <c r="G71" s="87"/>
+      <c r="H71" s="87"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="72" s="5">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H72" s="1"/>
     </row>
@@ -3315,8 +3227,8 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="29"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="28"/>
       <c r="H73" s="1"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="74" s="5">
@@ -4352,7 +4264,7 @@
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
-      <c r="I144" s="29"/>
+      <c r="I144" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="145" s="5">
       <c r="A145" s="1"/>
@@ -4363,7 +4275,7 @@
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
-      <c r="I145" s="29"/>
+      <c r="I145" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="146" s="5">
       <c r="A146" s="1"/>
@@ -4374,7 +4286,7 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
-      <c r="I146" s="29"/>
+      <c r="I146" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="147" s="5">
       <c r="A147" s="1"/>
@@ -4385,7 +4297,7 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
-      <c r="I147" s="29"/>
+      <c r="I147" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="148" s="5">
       <c r="A148" s="1"/>
@@ -4396,7 +4308,7 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
-      <c r="I148" s="29"/>
+      <c r="I148" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="8.1" outlineLevel="0" r="149" s="5">
       <c r="A149" s="1"/>
@@ -4407,7 +4319,7 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
-      <c r="I149" s="29"/>
+      <c r="I149" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="81" outlineLevel="0" r="150" s="5">
       <c r="A150" s="1"/>
@@ -4418,7 +4330,7 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
-      <c r="I150" s="29"/>
+      <c r="I150" s="28"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="3.75" outlineLevel="0" r="151" s="5">
       <c r="A151" s="1"/>
@@ -4450,54 +4362,54 @@
       <c r="J154" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="156">
-      <c r="I156" s="90"/>
-      <c r="J156" s="90"/>
+      <c r="I156" s="81"/>
+      <c r="J156" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="157">
-      <c r="I157" s="90"/>
-      <c r="J157" s="90"/>
+      <c r="I157" s="81"/>
+      <c r="J157" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="158">
-      <c r="I158" s="90"/>
-      <c r="J158" s="90"/>
+      <c r="I158" s="81"/>
+      <c r="J158" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="159">
-      <c r="I159" s="90"/>
-      <c r="J159" s="90"/>
+      <c r="I159" s="81"/>
+      <c r="J159" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="160">
-      <c r="I160" s="90"/>
-      <c r="J160" s="90"/>
+      <c r="I160" s="81"/>
+      <c r="J160" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="161">
-      <c r="I161" s="90"/>
-      <c r="J161" s="90"/>
+      <c r="I161" s="81"/>
+      <c r="J161" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="162">
-      <c r="I162" s="90"/>
-      <c r="J162" s="90"/>
+      <c r="I162" s="81"/>
+      <c r="J162" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="163">
-      <c r="I163" s="90"/>
-      <c r="J163" s="90"/>
+      <c r="I163" s="81"/>
+      <c r="J163" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="164">
-      <c r="I164" s="90"/>
-      <c r="J164" s="90"/>
+      <c r="I164" s="81"/>
+      <c r="J164" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="165">
-      <c r="I165" s="90"/>
-      <c r="J165" s="90"/>
+      <c r="I165" s="81"/>
+      <c r="J165" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="176">
-      <c r="I176" s="90"/>
+      <c r="I176" s="81"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="180">
-      <c r="I180" s="96"/>
+      <c r="I180" s="87"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="181">
       <c r="I181" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4577,347 +4489,347 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+      <c r="A3" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="88" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="97" t="s">
+      <c r="I3" s="88" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="88" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97" t="s">
+      <c r="L3" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97" t="s">
+      <c r="P3" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="97" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="97" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="97" t="s">
-        <v>75</v>
-      </c>
-      <c r="L3" s="97" t="s">
-        <v>76</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="98" t="n">
+      <c r="A4" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B4" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" s="98" t="n">
+      <c r="B4" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="89" t="n">
         <f aca="false">'Insertion Order'!D29</f>
         <v>0</v>
       </c>
-      <c r="H4" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="I4" s="100" t="inlineStr">
+      <c r="H4" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J4" s="100" t="inlineStr">
+      <c r="J4" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K4" s="99" t="str">
+      <c r="K4" s="90" t="str">
         <f aca="false">CONCATENATE(B4,C4,E4,F4,H4)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=300x250</v>
       </c>
-      <c r="L4" s="99" t="str">
+      <c r="L4" s="90" t="str">
         <f aca="false">CONCATENATE(B4,D4,E4,F4,H4)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=300x250</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="98" t="n">
+      <c r="A5" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B5" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G5" s="98" t="n">
+      <c r="B5" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="89" t="n">
         <f aca="false">'Insertion Order'!D29</f>
         <v>0</v>
       </c>
-      <c r="H5" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="100" t="inlineStr">
+      <c r="H5" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J5" s="100" t="inlineStr">
+      <c r="J5" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K5" s="99" t="str">
+      <c r="K5" s="90" t="str">
         <f aca="false">CONCATENATE(B5,C5,E5,F5,H5)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=728x90</v>
       </c>
-      <c r="L5" s="99" t="str">
+      <c r="L5" s="90" t="str">
         <f aca="false">CONCATENATE(B5,D5,E5,F5,H5)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=728x90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="98" t="n">
+      <c r="A6" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B6" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G6" s="98" t="n">
+      <c r="B6" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="89" t="n">
         <f aca="false">'Insertion Order'!D29</f>
         <v>0</v>
       </c>
-      <c r="H6" s="98" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="100" t="inlineStr">
+      <c r="H6" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J6" s="100" t="inlineStr">
+      <c r="J6" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K6" s="99" t="str">
+      <c r="K6" s="90" t="str">
         <f aca="false">CONCATENATE(B6,C6,E6,F6,H6)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=160x600</v>
       </c>
-      <c r="L6" s="99" t="str">
+      <c r="L6" s="90" t="str">
         <f aca="false">CONCATENATE(B6,D6,E6,F6,H6)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
-      <c r="A7" s="98" t="n">
+      <c r="A7" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B7" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="98" t="n">
+      <c r="B7" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="89" t="n">
         <f aca="false">'Insertion Order'!D30</f>
         <v>0</v>
       </c>
-      <c r="H7" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="I7" s="100" t="inlineStr">
+      <c r="H7" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J7" s="100" t="inlineStr">
+      <c r="J7" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K7" s="99" t="str">
+      <c r="K7" s="90" t="str">
         <f aca="false">CONCATENATE(B7,C7,E7,F7,H7)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=300x250</v>
       </c>
-      <c r="L7" s="99" t="str">
+      <c r="L7" s="90" t="str">
         <f aca="false">CONCATENATE(B7,D7,E7,F7,H7)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=300x250</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
-      <c r="A8" s="98" t="n">
+      <c r="A8" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B8" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="101"/>
-      <c r="F8" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="98" t="n">
+      <c r="B8" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="92"/>
+      <c r="F8" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="89" t="n">
         <f aca="false">'Insertion Order'!D30</f>
         <v>0</v>
       </c>
-      <c r="H8" s="98" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="100" t="inlineStr">
+      <c r="H8" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J8" s="100" t="inlineStr">
+      <c r="J8" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K8" s="99" t="str">
+      <c r="K8" s="90" t="str">
         <f aca="false">CONCATENATE(B8,C8,E8,F8,H8)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=728x90</v>
       </c>
-      <c r="L8" s="99" t="str">
+      <c r="L8" s="90" t="str">
         <f aca="false">CONCATENATE(B8,D8,E8,F8,H8)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=728x90</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="98" t="n">
+      <c r="A9" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
       </c>
-      <c r="B9" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="99" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="99" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="98" t="n">
+      <c r="B9" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="89" t="n">
         <f aca="false">'Insertion Order'!D30</f>
         <v>0</v>
       </c>
-      <c r="H9" s="98" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="100" t="inlineStr">
+      <c r="H9" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J9" s="100" t="inlineStr">
+      <c r="J9" s="91" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="K9" s="99" t="str">
+      <c r="K9" s="90" t="str">
         <f aca="false">CONCATENATE(B9,C9,E9,F9,H9)</f>
         <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=160x600</v>
       </c>
-      <c r="L9" s="99" t="str">
+      <c r="L9" s="90" t="str">
         <f aca="false">CONCATENATE(B9,D9,E9,F9,H9)</f>
         <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=160x600</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="R10" s="97" t="s">
-        <v>88</v>
+      <c r="R10" s="88" t="s">
+        <v>84</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
-      <c r="R11" s="98" t="s">
-        <v>82</v>
+      <c r="R11" s="89" t="s">
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
-      <c r="R12" s="98" t="s">
-        <v>84</v>
+      <c r="R12" s="89" t="s">
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
-      <c r="R13" s="98" t="s">
-        <v>85</v>
+      <c r="R13" s="89" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4958,386 +4870,384 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="102" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="103" width="9.70918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="103" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="103" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="103" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="103" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="103" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="103" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="103" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="102" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="93" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="94" width="9.70918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="94" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="94" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="94" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="94" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="94" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="94" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="94" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="93" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="104"/>
-      <c r="D3" s="105" t="s">
+      <c r="C3" s="95"/>
+      <c r="D3" s="96" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="I3" s="97"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="101">
+      <c r="A5" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="I3" s="106"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="110">
-      <c r="A5" s="107" t="s">
+      <c r="F5" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="107" t="s">
+      <c r="G5" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="H5" s="99" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="I5" s="98" t="s">
         <v>93</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="J5" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="K5" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="108" t="s">
+      <c r="L5" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="M5" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="J5" s="107" t="s">
+      <c r="N5" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="107" t="s">
+      <c r="O5" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="L5" s="107" t="s">
+      <c r="P5" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="M5" s="108" t="s">
+      <c r="Q5" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="N5" s="108" t="s">
+      <c r="R5" s="100"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="104"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
+      <c r="A7" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="O5" s="108" t="s">
+      <c r="B7" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="P5" s="108" t="s">
+      <c r="C7" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="Q5" s="107" t="s">
+      <c r="D7" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="R5" s="109"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="111" t="s">
+      <c r="F7" s="105" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="112"/>
-      <c r="R6" s="113"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="121">
-      <c r="A7" s="114" t="s">
+      <c r="G7" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="114" t="s">
+      <c r="H7" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="J7" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="114" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="114" t="s">
+      <c r="K7" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="L7" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="115" t="s">
+      <c r="M7" s="107" t="n">
+        <v>20</v>
+      </c>
+      <c r="N7" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="116" t="n">
+      <c r="O7" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="P7" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="110"/>
+      <c r="R7" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="112">
+      <c r="A8" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8" s="107" t="n">
         <v>8</v>
       </c>
-      <c r="I7" s="115" t="s">
+      <c r="I8" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="K8" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="M8" s="107" t="n">
+        <v>20</v>
+      </c>
+      <c r="N8" s="108" t="s">
+        <v>112</v>
+      </c>
+      <c r="O8" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="J7" s="115" t="s">
+      <c r="P8" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="K7" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="L7" s="114" t="s">
+      <c r="Q8" s="110"/>
+      <c r="R8" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="112">
+      <c r="A9" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="M7" s="116" t="n">
+      <c r="D9" s="105" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="L9" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="M9" s="107" t="n">
         <v>20</v>
       </c>
-      <c r="N7" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="O7" s="116" t="s">
+      <c r="N9" s="108" t="s">
+        <v>112</v>
+      </c>
+      <c r="O9" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="P9" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="112">
+      <c r="A10" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="P7" s="118" t="s">
+      <c r="D10" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="J10" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="L10" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="M10" s="107" t="n">
+        <v>20</v>
+      </c>
+      <c r="N10" s="108" t="s">
+        <v>112</v>
+      </c>
+      <c r="O10" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="P10" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="112">
+      <c r="A11" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" s="119"/>
-      <c r="R7" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="121">
-      <c r="A8" s="114" t="s">
+      <c r="D11" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="114" t="s">
+      <c r="H11" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="I11" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="115" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="114" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="114" t="s">
+      <c r="J11" s="106" t="s">
+        <v>109</v>
+      </c>
+      <c r="K11" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="114" t="s">
+      <c r="L11" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="115" t="s">
+      <c r="M11" s="107" t="n">
+        <v>20</v>
+      </c>
+      <c r="N11" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="I8" s="115" t="s">
+      <c r="O11" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="115" t="s">
+      <c r="P11" s="109" t="s">
         <v>114</v>
       </c>
-      <c r="K8" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="L8" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="M8" s="116" t="n">
-        <v>20</v>
-      </c>
-      <c r="N8" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="O8" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="P8" s="118" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q8" s="119"/>
-      <c r="R8" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="121">
-      <c r="A9" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="115" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="114" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="H9" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="I9" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="J9" s="115" t="s">
-        <v>114</v>
-      </c>
-      <c r="K9" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="L9" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="M9" s="116" t="n">
-        <v>20</v>
-      </c>
-      <c r="N9" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="O9" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="P9" s="118" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q9" s="119"/>
-      <c r="R9" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="121">
-      <c r="A10" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="115" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="114" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="114" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="H10" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="I10" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="J10" s="115" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="L10" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="M10" s="116" t="n">
-        <v>20</v>
-      </c>
-      <c r="N10" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="O10" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="P10" s="118" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q10" s="119"/>
-      <c r="R10" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="121">
-      <c r="A11" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="115" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="114" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="114" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="H11" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="I11" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" s="115" t="s">
-        <v>114</v>
-      </c>
-      <c r="K11" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="L11" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="M11" s="116" t="n">
-        <v>20</v>
-      </c>
-      <c r="N11" s="117" t="s">
-        <v>117</v>
-      </c>
-      <c r="O11" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="P11" s="118" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q11" s="119"/>
-      <c r="R11" s="120"/>
+      <c r="Q11" s="110"/>
+      <c r="R11" s="111"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="122"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="123"/>
-      <c r="O12" s="123"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="124"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
+      <c r="L12" s="114"/>
+      <c r="M12" s="114"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="114"/>
+      <c r="P12" s="114"/>
+      <c r="Q12" s="114"/>
+      <c r="R12" s="115"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5371,565 +5281,563 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="102" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="103" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="103" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="103" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="103" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="103" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="103" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="103" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="103" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="24" min="20" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="103" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="103" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="102" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="93" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="94" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="94" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="94" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="94" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="94" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="94" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="94" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="94" width="20.7091836734694"/>
+    <col collapsed="false" hidden="false" max="24" min="20" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="94" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="94" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="93" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="104"/>
-      <c r="D3" s="105" t="s">
+      <c r="C3" s="95"/>
+      <c r="D3" s="96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="101">
+      <c r="A5" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="98" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" s="98" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" s="98" t="s">
+        <v>93</v>
+      </c>
+      <c r="L5" s="98" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="98" t="s">
+        <v>96</v>
+      </c>
+      <c r="N5" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="O5" s="99" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="110">
-      <c r="A5" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="107" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="107" t="s">
+      <c r="P5" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="Q5" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="R5" s="99" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="107" t="s">
+      <c r="S5" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="I5" s="107" t="s">
-        <v>95</v>
-      </c>
-      <c r="J5" s="108" t="s">
-        <v>96</v>
-      </c>
-      <c r="K5" s="107" t="s">
-        <v>97</v>
-      </c>
-      <c r="L5" s="107" t="s">
+      <c r="T5" s="99" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" s="99" t="s">
+        <v>132</v>
+      </c>
+      <c r="V5" s="98" t="s">
+        <v>133</v>
+      </c>
+      <c r="W5" s="99" t="s">
+        <v>134</v>
+      </c>
+      <c r="X5" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="M5" s="107" t="s">
+      <c r="Y5" s="99" t="s">
         <v>100</v>
       </c>
-      <c r="N5" s="108" t="s">
+      <c r="Z5" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="O5" s="108" t="s">
-        <v>131</v>
-      </c>
-      <c r="P5" s="108" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q5" s="108" t="s">
-        <v>133</v>
-      </c>
-      <c r="R5" s="108" t="s">
-        <v>134</v>
-      </c>
-      <c r="S5" s="108" t="s">
+      <c r="AA5" s="100"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
+      <c r="A6" s="102"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="103"/>
+      <c r="Q6" s="103"/>
+      <c r="R6" s="103"/>
+      <c r="S6" s="103"/>
+      <c r="T6" s="103"/>
+      <c r="U6" s="103"/>
+      <c r="V6" s="103"/>
+      <c r="W6" s="103"/>
+      <c r="X6" s="103"/>
+      <c r="Y6" s="103"/>
+      <c r="Z6" s="103"/>
+      <c r="AA6" s="104"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
+      <c r="A7" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="106" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="105" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="T5" s="108" t="s">
+      <c r="H7" s="105" t="s">
         <v>136</v>
       </c>
-      <c r="U5" s="108" t="s">
+      <c r="I7" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="K7" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="N7" s="107" t="n">
+        <v>24</v>
+      </c>
+      <c r="O7" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="V5" s="107" t="s">
+      <c r="P7" s="107" t="s">
         <v>138</v>
       </c>
-      <c r="W5" s="108" t="s">
+      <c r="Q7" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="X5" s="108" t="s">
+      <c r="R7" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="S7" s="116" t="s">
+        <v>140</v>
+      </c>
+      <c r="T7" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="U7" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="V7" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="W7" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="X7" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y7" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z7" s="110"/>
+      <c r="AA7" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="112">
+      <c r="A8" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="Y5" s="108" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z5" s="107" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA5" s="109"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="111" t="s">
+      <c r="C8" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="105" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="105" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="112"/>
-      <c r="Q6" s="112"/>
-      <c r="R6" s="112"/>
-      <c r="S6" s="112"/>
-      <c r="T6" s="112"/>
-      <c r="U6" s="112"/>
-      <c r="V6" s="112"/>
-      <c r="W6" s="112"/>
-      <c r="X6" s="112"/>
-      <c r="Y6" s="112"/>
-      <c r="Z6" s="112"/>
-      <c r="AA6" s="113"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="121">
-      <c r="A7" s="114" t="s">
+      <c r="F8" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="114" t="s">
+      <c r="J8" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="K8" s="106" t="s">
         <v>108</v>
       </c>
-      <c r="C7" s="115" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="114" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="114" t="s">
+      <c r="L8" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="N8" s="107" t="n">
+        <v>24</v>
+      </c>
+      <c r="O8" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="S8" s="116" t="s">
+        <v>140</v>
+      </c>
+      <c r="T8" s="107" t="s">
+        <v>145</v>
+      </c>
+      <c r="U8" s="107" t="s">
+        <v>146</v>
+      </c>
+      <c r="V8" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="W8" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="X8" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y8" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z8" s="110"/>
+      <c r="AA8" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="112">
+      <c r="A9" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="105" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="114" t="s">
+      <c r="N9" s="107" t="n">
+        <v>24</v>
+      </c>
+      <c r="O9" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="P9" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q9" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="R9" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="S9" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="H7" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="I7" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="J7" s="116" t="n">
+      <c r="T9" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="U9" s="107" t="s">
+        <v>146</v>
+      </c>
+      <c r="V9" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="W9" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="X9" s="107" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y9" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z9" s="110"/>
+      <c r="AA9" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="112">
+      <c r="A10" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="105" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" s="107" t="n">
         <v>8</v>
       </c>
-      <c r="K7" s="115" t="s">
+      <c r="K10" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="N10" s="107" t="n">
+        <v>24</v>
+      </c>
+      <c r="O10" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="P10" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q10" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="R10" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="S10" s="116" t="s">
+        <v>140</v>
+      </c>
+      <c r="T10" s="107" t="s">
+        <v>148</v>
+      </c>
+      <c r="U10" s="107" t="s">
+        <v>146</v>
+      </c>
+      <c r="V10" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="W10" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="X10" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="M7" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="N7" s="116" t="n">
+      <c r="Y10" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z10" s="110"/>
+      <c r="AA10" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="112">
+      <c r="A11" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="105" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="105" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="105" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="106" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="107" t="n">
+        <v>8</v>
+      </c>
+      <c r="K11" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="105" t="s">
+        <v>110</v>
+      </c>
+      <c r="M11" s="105" t="s">
+        <v>111</v>
+      </c>
+      <c r="N11" s="118" t="n">
         <v>24</v>
       </c>
-      <c r="O7" s="117" t="s">
+      <c r="O11" s="119" t="s">
+        <v>137</v>
+      </c>
+      <c r="P11" s="107" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q11" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="R11" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="S11" s="116" t="s">
+        <v>140</v>
+      </c>
+      <c r="T11" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="U11" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="P7" s="116" t="s">
+      <c r="V11" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="Q7" s="117" t="s">
+      <c r="W11" s="108" t="s">
         <v>144</v>
       </c>
-      <c r="R7" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="S7" s="125" t="s">
-        <v>145</v>
-      </c>
-      <c r="T7" s="116" t="s">
-        <v>146</v>
-      </c>
-      <c r="U7" s="116" t="s">
-        <v>147</v>
-      </c>
-      <c r="V7" s="115" t="s">
-        <v>148</v>
-      </c>
-      <c r="W7" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="X7" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y7" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z7" s="119"/>
-      <c r="AA7" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="121">
-      <c r="A8" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="115" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="114" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="F8" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="H8" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="I8" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="J8" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="K8" s="115" t="s">
+      <c r="X11" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="L8" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="M8" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="N8" s="116" t="n">
-        <v>24</v>
-      </c>
-      <c r="O8" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="P8" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q8" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="R8" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="S8" s="125" t="s">
-        <v>145</v>
-      </c>
-      <c r="T8" s="116" t="s">
-        <v>150</v>
-      </c>
-      <c r="U8" s="116" t="s">
-        <v>151</v>
-      </c>
-      <c r="V8" s="115" t="s">
-        <v>148</v>
-      </c>
-      <c r="W8" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="X8" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y8" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z8" s="119"/>
-      <c r="AA8" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="121">
-      <c r="A9" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="115" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="114" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="F9" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="I9" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="J9" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="K9" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="L9" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="M9" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="N9" s="116" t="n">
-        <v>24</v>
-      </c>
-      <c r="O9" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="P9" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q9" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="R9" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="S9" s="125" t="s">
-        <v>145</v>
-      </c>
-      <c r="T9" s="116" t="s">
-        <v>152</v>
-      </c>
-      <c r="U9" s="116" t="s">
-        <v>151</v>
-      </c>
-      <c r="V9" s="115" t="s">
-        <v>148</v>
-      </c>
-      <c r="W9" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="X9" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y9" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z9" s="119"/>
-      <c r="AA9" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="121">
-      <c r="A10" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="115" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="114" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="F10" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="H10" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="I10" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="K10" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="M10" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="N10" s="116" t="n">
-        <v>24</v>
-      </c>
-      <c r="O10" s="117" t="s">
-        <v>142</v>
-      </c>
-      <c r="P10" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q10" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="R10" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="S10" s="125" t="s">
-        <v>145</v>
-      </c>
-      <c r="T10" s="116" t="s">
-        <v>153</v>
-      </c>
-      <c r="U10" s="116" t="s">
-        <v>151</v>
-      </c>
-      <c r="V10" s="115" t="s">
-        <v>148</v>
-      </c>
-      <c r="W10" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="X10" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y10" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z10" s="119"/>
-      <c r="AA10" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="121">
-      <c r="A11" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="114" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="115" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" s="114" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="114" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="114" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="114" t="s">
-        <v>141</v>
-      </c>
-      <c r="I11" s="115" t="s">
-        <v>112</v>
-      </c>
-      <c r="J11" s="116" t="n">
-        <v>8</v>
-      </c>
-      <c r="K11" s="115" t="s">
-        <v>113</v>
-      </c>
-      <c r="L11" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="M11" s="114" t="s">
-        <v>116</v>
-      </c>
-      <c r="N11" s="127" t="n">
-        <v>24</v>
-      </c>
-      <c r="O11" s="128" t="s">
-        <v>142</v>
-      </c>
-      <c r="P11" s="116" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q11" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="R11" s="117" t="s">
-        <v>144</v>
-      </c>
-      <c r="S11" s="125" t="s">
-        <v>145</v>
-      </c>
-      <c r="T11" s="116" t="s">
-        <v>154</v>
-      </c>
-      <c r="U11" s="116" t="s">
-        <v>147</v>
-      </c>
-      <c r="V11" s="115" t="s">
-        <v>148</v>
-      </c>
-      <c r="W11" s="117" t="s">
-        <v>149</v>
-      </c>
-      <c r="X11" s="116" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y11" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="120"/>
+      <c r="Y11" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z11" s="110"/>
+      <c r="AA11" s="111"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="122"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="123"/>
-      <c r="G12" s="123"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="123"/>
-      <c r="O12" s="123"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="123"/>
-      <c r="S12" s="123"/>
-      <c r="T12" s="123"/>
-      <c r="U12" s="123"/>
-      <c r="V12" s="123"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="123"/>
-      <c r="Y12" s="123"/>
-      <c r="Z12" s="123"/>
-      <c r="AA12" s="124"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
+      <c r="L12" s="114"/>
+      <c r="M12" s="114"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="114"/>
+      <c r="P12" s="114"/>
+      <c r="Q12" s="114"/>
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
+      <c r="U12" s="114"/>
+      <c r="V12" s="114"/>
+      <c r="W12" s="114"/>
+      <c r="X12" s="114"/>
+      <c r="Y12" s="114"/>
+      <c r="Z12" s="114"/>
+      <c r="AA12" s="115"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5963,207 +5871,205 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="102" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="103" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="103" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="103" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="103" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="103" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="102" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="93" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="94" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="94" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="94" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="94" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="94" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="93" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="120" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="101">
+      <c r="A5" s="98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="98" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" s="98" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="98" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="98" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="110">
-      <c r="A5" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="131" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="107" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="107" t="s">
+      <c r="J5" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="K5" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="G5" s="107" t="s">
+      <c r="L5" s="99" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="107" t="s">
+      <c r="M5" s="99" t="s">
+        <v>99</v>
+      </c>
+      <c r="N5" s="99" t="s">
+        <v>100</v>
+      </c>
+      <c r="O5" s="98" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" s="100"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
+      <c r="A6" s="102"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="103"/>
+      <c r="D6" s="103"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="104"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
+      <c r="A7" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="123" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="107" t="s">
+      <c r="C7" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="J5" s="108" t="s">
+      <c r="D7" s="105" t="s">
         <v>161</v>
       </c>
-      <c r="K5" s="108" t="s">
+      <c r="E7" s="105" t="s">
         <v>162</v>
       </c>
-      <c r="L5" s="108" t="s">
+      <c r="F7" s="105" t="s">
         <v>163</v>
       </c>
-      <c r="M5" s="108" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="108" t="s">
-        <v>104</v>
-      </c>
-      <c r="O5" s="107" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5" s="109"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="111" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
-      <c r="N6" s="112"/>
-      <c r="O6" s="112"/>
-      <c r="P6" s="113"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="121">
-      <c r="A7" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="132" t="s">
+      <c r="G7" s="105" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="H7" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="114" t="s">
+      <c r="I7" s="105" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="114" t="s">
+      <c r="J7" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="K7" s="107" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="G7" s="114" t="s">
+      <c r="M7" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="H7" s="114" t="s">
+      <c r="N7" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="O7" s="124" t="s">
         <v>170</v>
       </c>
-      <c r="I7" s="114" t="s">
+      <c r="P7" s="111"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8" s="112">
+      <c r="A8" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="123" t="s">
         <v>171</v>
       </c>
-      <c r="J7" s="116" t="s">
+      <c r="C8" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="K7" s="116" t="s">
-        <v>82</v>
-      </c>
-      <c r="L7" s="117" t="s">
+      <c r="D8" s="105" t="s">
         <v>173</v>
       </c>
-      <c r="M7" s="116" t="s">
-        <v>174</v>
-      </c>
-      <c r="N7" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="O7" s="133" t="s">
-        <v>175</v>
-      </c>
-      <c r="P7" s="120"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8" s="121">
-      <c r="A8" s="114" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="132" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="115" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="114" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="134" t="s">
+      <c r="E8" s="125" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="125" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="125" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="105" t="s">
+        <v>166</v>
+      </c>
+      <c r="J8" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="F8" s="114" t="s">
+      <c r="K8" s="107" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="108" t="s">
         <v>168</v>
       </c>
-      <c r="G8" s="134" t="s">
+      <c r="M8" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="H8" s="134" t="s">
+      <c r="N8" s="117" t="s">
+        <v>114</v>
+      </c>
+      <c r="O8" s="124" t="s">
         <v>170</v>
       </c>
-      <c r="I8" s="114" t="s">
-        <v>171</v>
-      </c>
-      <c r="J8" s="116" t="s">
-        <v>172</v>
-      </c>
-      <c r="K8" s="116" t="s">
-        <v>82</v>
-      </c>
-      <c r="L8" s="117" t="s">
-        <v>173</v>
-      </c>
-      <c r="M8" s="116" t="s">
-        <v>174</v>
-      </c>
-      <c r="N8" s="126" t="s">
-        <v>119</v>
-      </c>
-      <c r="O8" s="133" t="s">
-        <v>175</v>
-      </c>
-      <c r="P8" s="120"/>
+      <c r="P8" s="111"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="9">
-      <c r="A9" s="122"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="123"/>
-      <c r="O9" s="123"/>
-      <c r="P9" s="124"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="114"/>
+      <c r="P9" s="115"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
parsing and displaying of Creatives
</commit_message>
<xml_diff>
--- a/spec/fixtures/io_files/Collective_IO.xlsx
+++ b/spec/fixtures/io_files/Collective_IO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Insertion Order" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,10 +21,13 @@
     <definedName function="false" hidden="false" name="Network" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Standard Specs'!$A$1:$Q$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Rich Media Specs'!$A$1:$Z$11</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Video Specs'!$A$1:$O$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -583,7 +586,7 @@
     <numFmt formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)" numFmtId="170"/>
     <numFmt formatCode="@" numFmtId="171"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -727,6 +730,11 @@
       <color rgb="FF0000FF"/>
       <sz val="11"/>
       <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -933,7 +941,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1298,6 +1306,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1318,7 +1330,7 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1342,7 +1354,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1354,35 +1366,35 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="25" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="26" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="22" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="23" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1398,27 +1410,27 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="23" numFmtId="171" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="2" fontId="24" numFmtId="171" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="24" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="3" fillId="2" fontId="25" numFmtId="164" xfId="20">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="13" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="21" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="22" numFmtId="164" xfId="21">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1426,15 +1438,15 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="23" numFmtId="164" xfId="20">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="1" fillId="2" fontId="24" numFmtId="164" xfId="20">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="23" numFmtId="164" xfId="21">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="2" fontId="24" numFmtId="164" xfId="21">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1447,7 +1459,7 @@
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
     <cellStyle builtinId="8" customBuiltin="false" name="*unknown*" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Normal 2" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Normal 2" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1517,15 +1529,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>158760</xdr:colOff>
+      <xdr:colOff>185760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>67680</xdr:rowOff>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>391680</xdr:colOff>
+      <xdr:colOff>418320</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1540,8 +1552,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="158760" y="210240"/>
-          <a:ext cx="1230840" cy="599400"/>
+          <a:off x="185760" y="201240"/>
+          <a:ext cx="1230480" cy="599040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1553,15 +1565,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1281960</xdr:colOff>
+      <xdr:colOff>1308600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1570,8 +1582,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="48600"/>
-          <a:ext cx="12354840" cy="46800"/>
+          <a:off x="81000" y="39600"/>
+          <a:ext cx="12354480" cy="46440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1592,15 +1604,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1281960</xdr:colOff>
+      <xdr:colOff>1308600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>19440</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1609,8 +1621,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="877320"/>
-          <a:ext cx="12354840" cy="46800"/>
+          <a:off x="81000" y="868320"/>
+          <a:ext cx="12354480" cy="46440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1631,15 +1643,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>81000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1320120</xdr:colOff>
+      <xdr:colOff>1346760</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>149760</xdr:rowOff>
+      <xdr:rowOff>140400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1648,8 +1660,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="6209280"/>
-          <a:ext cx="12393000" cy="142200"/>
+          <a:off x="81000" y="6200280"/>
+          <a:ext cx="12392640" cy="141840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1670,15 +1682,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>141120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1310760</xdr:colOff>
+      <xdr:colOff>1337400</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>24120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1687,8 +1699,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="54000" y="2963160"/>
-          <a:ext cx="12383640" cy="45000"/>
+          <a:off x="81000" y="2954160"/>
+          <a:ext cx="12383280" cy="44640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1714,15 +1726,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>111240</xdr:colOff>
+      <xdr:colOff>138240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>39240</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>177120</xdr:colOff>
+      <xdr:colOff>203760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>238680</xdr:rowOff>
+      <xdr:rowOff>229320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1737,8 +1749,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="111240" y="39240"/>
-          <a:ext cx="1597320" cy="723240"/>
+          <a:off x="138240" y="30240"/>
+          <a:ext cx="1596960" cy="722880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1755,15 +1767,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>158760</xdr:colOff>
+      <xdr:colOff>185760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>87480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>224640</xdr:colOff>
+      <xdr:colOff>251280</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>295920</xdr:rowOff>
+      <xdr:rowOff>286560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1778,8 +1790,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="158760" y="96480"/>
-          <a:ext cx="1597320" cy="723240"/>
+          <a:off x="185760" y="87480"/>
+          <a:ext cx="1596960" cy="722880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1796,15 +1808,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>158760</xdr:colOff>
+      <xdr:colOff>185760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>224640</xdr:colOff>
+      <xdr:colOff>251280</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>248040</xdr:rowOff>
+      <xdr:rowOff>238680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1819,8 +1831,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="158760" y="48600"/>
-          <a:ext cx="1597320" cy="723240"/>
+          <a:off x="185760" y="39600"/>
+          <a:ext cx="1596960" cy="722880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1839,7 +1851,7 @@
   </sheetPr>
   <dimension ref="A1:AI181"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -4467,8 +4479,8 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="H1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="L9" activeCellId="0" pane="topLeft" sqref="L9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I4" activeCellId="0" pane="topLeft" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4525,7 +4537,7 @@
         <v>73</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4">
       <c r="A4" s="89" t="n">
         <f aca="false">'Insertion Order'!C18</f>
         <v>0</v>
@@ -4539,6 +4551,9 @@
       <c r="D4" s="90" t="s">
         <v>76</v>
       </c>
+      <c r="E4" s="91" t="n">
+        <v>78002775</v>
+      </c>
       <c r="F4" s="89" t="s">
         <v>77</v>
       </c>
@@ -4549,13 +4564,13 @@
       <c r="H4" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="91" t="inlineStr">
+      <c r="I4" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J4" s="91" t="inlineStr">
+      <c r="J4" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4563,11 +4578,11 @@
       </c>
       <c r="K4" s="90" t="str">
         <f aca="false">CONCATENATE(B4,C4,E4,F4,H4)</f>
-        <v>http://ad.doubleclick.net/ad/.collective;adid=;sz=300x250</v>
+        <v>http://ad.doubleclick.net/ad/.collective;adid=78002775;sz=300x250</v>
       </c>
       <c r="L4" s="90" t="str">
         <f aca="false">CONCATENATE(B4,D4,E4,F4,H4)</f>
-        <v>http://ad.doubleclick.net/jump/.collective;adid=;sz=300x250</v>
+        <v>http://ad.doubleclick.net/jump/.collective;adid=78002775;sz=300x250</v>
       </c>
       <c r="P4" s="0" t="s">
         <v>79</v>
@@ -4598,13 +4613,13 @@
       <c r="H5" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="91" t="inlineStr">
+      <c r="I5" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J5" s="91" t="inlineStr">
+      <c r="J5" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4644,13 +4659,13 @@
       <c r="H6" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="91" t="inlineStr">
+      <c r="I6" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J6" s="91" t="inlineStr">
+      <c r="J6" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4693,13 +4708,13 @@
       <c r="H7" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="91" t="inlineStr">
+      <c r="I7" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J7" s="91" t="inlineStr">
+      <c r="J7" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4731,7 +4746,7 @@
       <c r="D8" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="92"/>
+      <c r="E8" s="93"/>
       <c r="F8" s="89" t="s">
         <v>77</v>
       </c>
@@ -4742,13 +4757,13 @@
       <c r="H8" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="I8" s="91" t="inlineStr">
+      <c r="I8" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J8" s="91" t="inlineStr">
+      <c r="J8" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4791,13 +4806,13 @@
       <c r="H9" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="91" t="inlineStr">
+      <c r="I9" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H25</f>
         <is>
           <t/>
         </is>
       </c>
-      <c r="J9" s="91" t="inlineStr">
+      <c r="J9" s="92" t="inlineStr">
         <f aca="false">'Insertion Order'!H26</f>
         <is>
           <t/>
@@ -4870,384 +4885,384 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="93" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="94" width="9.70918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="94" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="94" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="94" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="94" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="94" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="94" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="94" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="93" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="94" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="95" width="9.70918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="95" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="95" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="95" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="95" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="95" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="95" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="95" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="94" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="95"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="I3" s="97"/>
+      <c r="E3" s="98"/>
+      <c r="F3" s="98"/>
+      <c r="I3" s="98"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="101">
-      <c r="A5" s="98" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="102">
+      <c r="A5" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="99" t="s">
+      <c r="H5" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="98" t="s">
+      <c r="I5" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="98" t="s">
+      <c r="L5" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="99" t="s">
+      <c r="M5" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="99" t="s">
+      <c r="N5" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="O5" s="99" t="s">
+      <c r="O5" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="P5" s="99" t="s">
+      <c r="P5" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="Q5" s="98" t="s">
+      <c r="Q5" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="R5" s="100"/>
+      <c r="R5" s="101"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="104"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
-      <c r="A7" s="105" t="s">
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="104"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="105"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="113">
+      <c r="A7" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="107" t="n">
+      <c r="H7" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="106" t="s">
+      <c r="J7" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K7" s="105" t="s">
+      <c r="K7" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L7" s="105" t="s">
+      <c r="L7" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="M7" s="107" t="n">
+      <c r="M7" s="108" t="n">
         <v>20</v>
       </c>
-      <c r="N7" s="108" t="s">
+      <c r="N7" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="O7" s="107" t="s">
+      <c r="O7" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="P7" s="109" t="s">
+      <c r="P7" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="112">
-      <c r="A8" s="105" t="s">
+      <c r="Q7" s="111"/>
+      <c r="R7" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="113">
+      <c r="A8" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="106" t="s">
+      <c r="C8" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="106" t="s">
+      <c r="G8" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="H8" s="107" t="n">
+      <c r="H8" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="I8" s="106" t="s">
+      <c r="I8" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="106" t="s">
+      <c r="J8" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K8" s="105" t="s">
+      <c r="K8" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L8" s="105" t="s">
+      <c r="L8" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="M8" s="107" t="n">
+      <c r="M8" s="108" t="n">
         <v>20</v>
       </c>
-      <c r="N8" s="108" t="s">
+      <c r="N8" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="O8" s="107" t="s">
+      <c r="O8" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="P8" s="109" t="s">
+      <c r="P8" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Q8" s="110"/>
-      <c r="R8" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="112">
-      <c r="A9" s="105" t="s">
+      <c r="Q8" s="111"/>
+      <c r="R8" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="113">
+      <c r="A9" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="105" t="s">
+      <c r="E9" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="106" t="s">
+      <c r="G9" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="107" t="n">
+      <c r="H9" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="J9" s="106" t="s">
+      <c r="J9" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="105" t="s">
+      <c r="K9" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="M9" s="107" t="n">
+      <c r="M9" s="108" t="n">
         <v>20</v>
       </c>
-      <c r="N9" s="108" t="s">
+      <c r="N9" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="O9" s="107" t="s">
+      <c r="O9" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="P9" s="109" t="s">
+      <c r="P9" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Q9" s="110"/>
-      <c r="R9" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="112">
-      <c r="A10" s="105" t="s">
+      <c r="Q9" s="111"/>
+      <c r="R9" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="113">
+      <c r="A10" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="105" t="s">
+      <c r="E10" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="105" t="s">
+      <c r="F10" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="107" t="n">
+      <c r="H10" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="106" t="s">
+      <c r="I10" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="J10" s="106" t="s">
+      <c r="J10" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="105" t="s">
+      <c r="K10" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L10" s="105" t="s">
+      <c r="L10" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="M10" s="107" t="n">
+      <c r="M10" s="108" t="n">
         <v>20</v>
       </c>
-      <c r="N10" s="108" t="s">
+      <c r="N10" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="O10" s="107" t="s">
+      <c r="O10" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="P10" s="109" t="s">
+      <c r="P10" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Q10" s="110"/>
-      <c r="R10" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="112">
-      <c r="A11" s="105" t="s">
+      <c r="Q10" s="111"/>
+      <c r="R10" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="113">
+      <c r="A11" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="105" t="s">
+      <c r="E11" s="106" t="s">
         <v>105</v>
       </c>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="107" t="n">
+      <c r="H11" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="I11" s="106" t="s">
+      <c r="I11" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="106" t="s">
+      <c r="J11" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K11" s="105" t="s">
+      <c r="K11" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="105" t="s">
+      <c r="L11" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="M11" s="107" t="n">
+      <c r="M11" s="108" t="n">
         <v>20</v>
       </c>
-      <c r="N11" s="108" t="s">
+      <c r="N11" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="O11" s="107" t="s">
+      <c r="O11" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="P11" s="109" t="s">
+      <c r="P11" s="110" t="s">
         <v>114</v>
       </c>
-      <c r="Q11" s="110"/>
-      <c r="R11" s="111"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="114"/>
-      <c r="L12" s="114"/>
-      <c r="M12" s="114"/>
-      <c r="N12" s="114"/>
-      <c r="O12" s="114"/>
-      <c r="P12" s="114"/>
-      <c r="Q12" s="114"/>
-      <c r="R12" s="115"/>
+      <c r="A12" s="114"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="115"/>
+      <c r="P12" s="115"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="116"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5281,563 +5296,563 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="93" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="94" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="94" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="94" width="10.7091836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="94" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="94" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="94" width="14.7040816326531"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="94" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="94" width="20.7091836734694"/>
-    <col collapsed="false" hidden="false" max="24" min="20" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="94" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="94" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="93" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="94" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="95" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="95" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="95" width="10.7091836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="95" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="13" style="95" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="95" width="14.7040816326531"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="95" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="95" width="20.7091836734694"/>
+    <col collapsed="false" hidden="false" max="24" min="20" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="95" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="95" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="94" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="95"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="97" t="s">
         <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="36" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="101">
-      <c r="A5" s="98" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="51.75" outlineLevel="0" r="5" s="102">
+      <c r="A5" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="99" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="99" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="99" t="s">
         <v>123</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="99" t="s">
         <v>124</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="98" t="s">
+      <c r="I5" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="99" t="s">
+      <c r="J5" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="98" t="s">
+      <c r="K5" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="L5" s="98" t="s">
+      <c r="L5" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="M5" s="98" t="s">
+      <c r="M5" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="N5" s="99" t="s">
+      <c r="N5" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="O5" s="99" t="s">
+      <c r="O5" s="100" t="s">
         <v>126</v>
       </c>
-      <c r="P5" s="99" t="s">
+      <c r="P5" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="Q5" s="99" t="s">
+      <c r="Q5" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="R5" s="99" t="s">
+      <c r="R5" s="100" t="s">
         <v>129</v>
       </c>
-      <c r="S5" s="99" t="s">
+      <c r="S5" s="100" t="s">
         <v>130</v>
       </c>
-      <c r="T5" s="99" t="s">
+      <c r="T5" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="U5" s="99" t="s">
+      <c r="U5" s="100" t="s">
         <v>132</v>
       </c>
-      <c r="V5" s="98" t="s">
+      <c r="V5" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="W5" s="99" t="s">
+      <c r="W5" s="100" t="s">
         <v>134</v>
       </c>
-      <c r="X5" s="99" t="s">
+      <c r="X5" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="99" t="s">
+      <c r="Y5" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="Z5" s="98" t="s">
+      <c r="Z5" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="AA5" s="100"/>
+      <c r="AA5" s="101"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="102"/>
-      <c r="B6" s="103"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="103"/>
-      <c r="Q6" s="103"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="103"/>
-      <c r="T6" s="103"/>
-      <c r="U6" s="103"/>
-      <c r="V6" s="103"/>
-      <c r="W6" s="103"/>
-      <c r="X6" s="103"/>
-      <c r="Y6" s="103"/>
-      <c r="Z6" s="103"/>
-      <c r="AA6" s="104"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
-      <c r="A7" s="105" t="s">
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="104"/>
+      <c r="Q6" s="104"/>
+      <c r="R6" s="104"/>
+      <c r="S6" s="104"/>
+      <c r="T6" s="104"/>
+      <c r="U6" s="104"/>
+      <c r="V6" s="104"/>
+      <c r="W6" s="104"/>
+      <c r="X6" s="104"/>
+      <c r="Y6" s="104"/>
+      <c r="Z6" s="104"/>
+      <c r="AA6" s="105"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="113">
+      <c r="A7" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="B7" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="105" t="s">
+      <c r="H7" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I7" s="106" t="s">
+      <c r="I7" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="J7" s="107" t="n">
+      <c r="J7" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="K7" s="106" t="s">
+      <c r="K7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L7" s="105" t="s">
+      <c r="L7" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="105" t="s">
+      <c r="M7" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="N7" s="107" t="n">
+      <c r="N7" s="108" t="n">
         <v>24</v>
       </c>
-      <c r="O7" s="108" t="s">
+      <c r="O7" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="P7" s="107" t="s">
+      <c r="P7" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="Q7" s="108" t="s">
+      <c r="Q7" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R7" s="108" t="s">
+      <c r="R7" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="S7" s="116" t="s">
+      <c r="S7" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="T7" s="107" t="s">
+      <c r="T7" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="U7" s="107" t="s">
+      <c r="U7" s="108" t="s">
         <v>142</v>
       </c>
-      <c r="V7" s="106" t="s">
+      <c r="V7" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="W7" s="108" t="s">
+      <c r="W7" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="X7" s="107" t="s">
+      <c r="X7" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="Y7" s="117" t="s">
+      <c r="Y7" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="Z7" s="110"/>
-      <c r="AA7" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="112">
-      <c r="A8" s="105" t="s">
+      <c r="Z7" s="111"/>
+      <c r="AA7" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="8" s="113">
+      <c r="A8" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="106" t="s">
+      <c r="C8" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="105" t="s">
+      <c r="E8" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G8" s="105" t="s">
+      <c r="G8" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="H8" s="105" t="s">
+      <c r="H8" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="106" t="s">
+      <c r="I8" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="107" t="n">
+      <c r="J8" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="K8" s="106" t="s">
+      <c r="K8" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L8" s="105" t="s">
+      <c r="L8" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="M8" s="105" t="s">
+      <c r="M8" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="N8" s="107" t="n">
+      <c r="N8" s="108" t="n">
         <v>24</v>
       </c>
-      <c r="O8" s="108" t="s">
+      <c r="O8" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="P8" s="107" t="s">
+      <c r="P8" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="Q8" s="108" t="s">
+      <c r="Q8" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R8" s="108" t="s">
+      <c r="R8" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="S8" s="116" t="s">
+      <c r="S8" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="T8" s="107" t="s">
+      <c r="T8" s="108" t="s">
         <v>145</v>
       </c>
-      <c r="U8" s="107" t="s">
+      <c r="U8" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="V8" s="106" t="s">
+      <c r="V8" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="W8" s="108" t="s">
+      <c r="W8" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="X8" s="107" t="s">
+      <c r="X8" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="Y8" s="117" t="s">
+      <c r="Y8" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="Z8" s="110"/>
-      <c r="AA8" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="112">
-      <c r="A9" s="105" t="s">
+      <c r="Z8" s="111"/>
+      <c r="AA8" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="9" s="113">
+      <c r="A9" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="107" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="105" t="s">
+      <c r="D9" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="105" t="s">
+      <c r="E9" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="F9" s="105" t="s">
+      <c r="F9" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="H9" s="105" t="s">
+      <c r="H9" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="106" t="s">
+      <c r="I9" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="J9" s="107" t="n">
+      <c r="J9" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="K9" s="106" t="s">
+      <c r="K9" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="M9" s="105" t="s">
+      <c r="M9" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="N9" s="107" t="n">
+      <c r="N9" s="108" t="n">
         <v>24</v>
       </c>
-      <c r="O9" s="108" t="s">
+      <c r="O9" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="P9" s="107" t="s">
+      <c r="P9" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="Q9" s="108" t="s">
+      <c r="Q9" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R9" s="108" t="s">
+      <c r="R9" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="S9" s="116" t="s">
+      <c r="S9" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="T9" s="107" t="s">
+      <c r="T9" s="108" t="s">
         <v>147</v>
       </c>
-      <c r="U9" s="107" t="s">
+      <c r="U9" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="V9" s="106" t="s">
+      <c r="V9" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="W9" s="108" t="s">
+      <c r="W9" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="X9" s="107" t="s">
+      <c r="X9" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="Y9" s="117" t="s">
+      <c r="Y9" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="Z9" s="110"/>
-      <c r="AA9" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="112">
-      <c r="A10" s="105" t="s">
+      <c r="Z9" s="111"/>
+      <c r="AA9" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="10" s="113">
+      <c r="A10" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="107" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="105" t="s">
+      <c r="D10" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="105" t="s">
+      <c r="E10" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="105" t="s">
+      <c r="F10" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G10" s="105" t="s">
+      <c r="G10" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="H10" s="105" t="s">
+      <c r="H10" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="106" t="s">
+      <c r="I10" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="107" t="n">
+      <c r="J10" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="K10" s="106" t="s">
+      <c r="K10" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L10" s="105" t="s">
+      <c r="L10" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="M10" s="105" t="s">
+      <c r="M10" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="N10" s="107" t="n">
+      <c r="N10" s="108" t="n">
         <v>24</v>
       </c>
-      <c r="O10" s="108" t="s">
+      <c r="O10" s="109" t="s">
         <v>137</v>
       </c>
-      <c r="P10" s="107" t="s">
+      <c r="P10" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="Q10" s="108" t="s">
+      <c r="Q10" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R10" s="108" t="s">
+      <c r="R10" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="S10" s="116" t="s">
+      <c r="S10" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="T10" s="107" t="s">
+      <c r="T10" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="U10" s="107" t="s">
+      <c r="U10" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="V10" s="106" t="s">
+      <c r="V10" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="W10" s="108" t="s">
+      <c r="W10" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="X10" s="107" t="s">
+      <c r="X10" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="Y10" s="117" t="s">
+      <c r="Y10" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="Z10" s="110"/>
-      <c r="AA10" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="112">
-      <c r="A11" s="105" t="s">
+      <c r="Z10" s="111"/>
+      <c r="AA10" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="11" s="113">
+      <c r="A11" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="105" t="s">
+      <c r="B11" s="106" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="107" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="105" t="s">
+      <c r="D11" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="105" t="s">
+      <c r="E11" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="105" t="s">
+      <c r="F11" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="105" t="s">
+      <c r="G11" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="105" t="s">
+      <c r="H11" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="106" t="s">
+      <c r="I11" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="J11" s="107" t="n">
+      <c r="J11" s="108" t="n">
         <v>8</v>
       </c>
-      <c r="K11" s="106" t="s">
+      <c r="K11" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L11" s="105" t="s">
+      <c r="L11" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="M11" s="105" t="s">
+      <c r="M11" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="N11" s="118" t="n">
+      <c r="N11" s="119" t="n">
         <v>24</v>
       </c>
-      <c r="O11" s="119" t="s">
+      <c r="O11" s="120" t="s">
         <v>137</v>
       </c>
-      <c r="P11" s="107" t="s">
+      <c r="P11" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="Q11" s="108" t="s">
+      <c r="Q11" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="R11" s="108" t="s">
+      <c r="R11" s="109" t="s">
         <v>139</v>
       </c>
-      <c r="S11" s="116" t="s">
+      <c r="S11" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="T11" s="107" t="s">
+      <c r="T11" s="108" t="s">
         <v>149</v>
       </c>
-      <c r="U11" s="107" t="s">
+      <c r="U11" s="108" t="s">
         <v>142</v>
       </c>
-      <c r="V11" s="106" t="s">
+      <c r="V11" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="W11" s="108" t="s">
+      <c r="W11" s="109" t="s">
         <v>144</v>
       </c>
-      <c r="X11" s="107" t="s">
+      <c r="X11" s="108" t="s">
         <v>113</v>
       </c>
-      <c r="Y11" s="117" t="s">
+      <c r="Y11" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="Z11" s="110"/>
-      <c r="AA11" s="111"/>
+      <c r="Z11" s="111"/>
+      <c r="AA11" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="12">
-      <c r="A12" s="113"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
-      <c r="D12" s="114"/>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="114"/>
-      <c r="K12" s="114"/>
-      <c r="L12" s="114"/>
-      <c r="M12" s="114"/>
-      <c r="N12" s="114"/>
-      <c r="O12" s="114"/>
-      <c r="P12" s="114"/>
-      <c r="Q12" s="114"/>
-      <c r="R12" s="114"/>
-      <c r="S12" s="114"/>
-      <c r="T12" s="114"/>
-      <c r="U12" s="114"/>
-      <c r="V12" s="114"/>
-      <c r="W12" s="114"/>
-      <c r="X12" s="114"/>
-      <c r="Y12" s="114"/>
-      <c r="Z12" s="114"/>
-      <c r="AA12" s="115"/>
+      <c r="A12" s="114"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
+      <c r="L12" s="115"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
+      <c r="O12" s="115"/>
+      <c r="P12" s="115"/>
+      <c r="Q12" s="115"/>
+      <c r="R12" s="115"/>
+      <c r="S12" s="115"/>
+      <c r="T12" s="115"/>
+      <c r="U12" s="115"/>
+      <c r="V12" s="115"/>
+      <c r="W12" s="115"/>
+      <c r="X12" s="115"/>
+      <c r="Y12" s="115"/>
+      <c r="Z12" s="115"/>
+      <c r="AA12" s="116"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5871,205 +5886,205 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="93" width="21.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="94" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="5" style="94" width="11.7091836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="94" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="94" width="25.7091836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="94" width="26.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="93" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="94" width="21.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="95" width="22.7040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="5" style="95" width="11.7091836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="95" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="95" width="25.7091836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="95" width="26.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="94" width="9.14285714285714"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="3">
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="121" t="s">
         <v>150</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="33.95" outlineLevel="0" r="4"/>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="101">
-      <c r="A5" s="98" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39" outlineLevel="0" r="5" s="102">
+      <c r="A5" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="98" t="s">
+      <c r="C5" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="E5" s="99" t="s">
         <v>151</v>
       </c>
-      <c r="F5" s="98" t="s">
+      <c r="F5" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="98" t="s">
+      <c r="G5" s="99" t="s">
         <v>153</v>
       </c>
-      <c r="H5" s="98" t="s">
+      <c r="H5" s="99" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="98" t="s">
+      <c r="I5" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="J5" s="99" t="s">
+      <c r="J5" s="100" t="s">
         <v>156</v>
       </c>
-      <c r="K5" s="99" t="s">
+      <c r="K5" s="100" t="s">
         <v>157</v>
       </c>
-      <c r="L5" s="99" t="s">
+      <c r="L5" s="100" t="s">
         <v>158</v>
       </c>
-      <c r="M5" s="99" t="s">
+      <c r="M5" s="100" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="99" t="s">
+      <c r="N5" s="100" t="s">
         <v>100</v>
       </c>
-      <c r="O5" s="98" t="s">
+      <c r="O5" s="99" t="s">
         <v>101</v>
       </c>
-      <c r="P5" s="100"/>
+      <c r="P5" s="101"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
-      <c r="A6" s="102"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
-      <c r="G6" s="103"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="103"/>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
-      <c r="L6" s="103"/>
-      <c r="M6" s="103"/>
-      <c r="N6" s="103"/>
-      <c r="O6" s="103"/>
-      <c r="P6" s="104"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="112">
-      <c r="A7" s="105" t="s">
+      <c r="A6" s="103"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="104"/>
+      <c r="N6" s="104"/>
+      <c r="O6" s="104"/>
+      <c r="P6" s="105"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="63.75" outlineLevel="0" r="7" s="113">
+      <c r="A7" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="124" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="106" t="s">
+      <c r="C7" s="107" t="s">
         <v>160</v>
       </c>
-      <c r="D7" s="105" t="s">
+      <c r="D7" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="106" t="s">
         <v>162</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="106" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="H7" s="105" t="s">
+      <c r="H7" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="I7" s="105" t="s">
+      <c r="I7" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="J7" s="107" t="s">
+      <c r="J7" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="K7" s="107" t="s">
+      <c r="K7" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="108" t="s">
+      <c r="L7" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="M7" s="107" t="s">
+      <c r="M7" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="N7" s="117" t="s">
+      <c r="N7" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="O7" s="124" t="s">
+      <c r="O7" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="P7" s="111"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8" s="112">
-      <c r="A8" s="105" t="s">
+      <c r="P7" s="112"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="64.5" outlineLevel="0" r="8" s="113">
+      <c r="A8" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="123" t="s">
+      <c r="B8" s="124" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="106" t="s">
+      <c r="C8" s="107" t="s">
         <v>172</v>
       </c>
-      <c r="D8" s="105" t="s">
+      <c r="D8" s="106" t="s">
         <v>173</v>
       </c>
-      <c r="E8" s="125" t="s">
+      <c r="E8" s="126" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="106" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="125" t="s">
+      <c r="G8" s="126" t="s">
         <v>164</v>
       </c>
-      <c r="H8" s="125" t="s">
+      <c r="H8" s="126" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="105" t="s">
+      <c r="I8" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="J8" s="107" t="s">
+      <c r="J8" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="K8" s="107" t="s">
+      <c r="K8" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="L8" s="108" t="s">
+      <c r="L8" s="109" t="s">
         <v>168</v>
       </c>
-      <c r="M8" s="107" t="s">
+      <c r="M8" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="N8" s="117" t="s">
+      <c r="N8" s="118" t="s">
         <v>114</v>
       </c>
-      <c r="O8" s="124" t="s">
+      <c r="O8" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="P8" s="111"/>
+      <c r="P8" s="112"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.5" outlineLevel="0" r="9">
-      <c r="A9" s="113"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="114"/>
-      <c r="O9" s="114"/>
-      <c r="P9" s="115"/>
+      <c r="A9" s="114"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="116"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>